<commit_message>
EUR Bond Framework final
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_020_BTPQuotes.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_020_BTPQuotes.xlsx
@@ -1085,7 +1085,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1134,9 +1134,9 @@
       <c r="E2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="31" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>#NAME?</v>
+      <c r="F2" s="31" t="str">
+        <f>_xll.ohRangeRetrieveError(D2)</f>
+        <v/>
       </c>
       <c r="G2" s="23"/>
     </row>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="D3" s="24" t="str">
         <f>IF(ISNA(B3),NA(),_xll.qlCompositeQuote($E3&amp;"-ResPrem"&amp;QuoteSuffix,E3&amp;QuoteSuffix,C3,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003080402-ResPrem_Quote#0000</v>
+        <v>IT0003080402-ResPrem_Quote#0001</v>
       </c>
       <c r="E3" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B3))</f>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D4" s="24" t="str">
         <f>IF(ISNA(B4),NA(),_xll.qlCompositeQuote($E4&amp;"-ResPrem"&amp;QuoteSuffix,E4&amp;QuoteSuffix,C4,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003190912-ResPrem_Quote#0000</v>
+        <v>IT0003190912-ResPrem_Quote#0001</v>
       </c>
       <c r="E4" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B4))</f>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D5" s="24" t="str">
         <f>IF(ISNA(B5),NA(),_xll.qlCompositeQuote($E5&amp;"-ResPrem"&amp;QuoteSuffix,E5&amp;QuoteSuffix,C5,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003357982-ResPrem_Quote#0000</v>
+        <v>IT0003357982-ResPrem_Quote#0001</v>
       </c>
       <c r="E5" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B5))</f>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D6" s="24" t="str">
         <f>IF(ISNA(B6),NA(),_xll.qlCompositeQuote($E6&amp;"-ResPrem"&amp;QuoteSuffix,E6&amp;QuoteSuffix,C6,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003472336-ResPrem_Quote#0000</v>
+        <v>IT0003472336-ResPrem_Quote#0001</v>
       </c>
       <c r="E6" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B6))</f>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="D7" s="24" t="str">
         <f>IF(ISNA(B7),NA(),_xll.qlCompositeQuote($E7&amp;"-ResPrem"&amp;QuoteSuffix,E7&amp;QuoteSuffix,C7,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003618383-ResPrem_Quote#0000</v>
+        <v>IT0003618383-ResPrem_Quote#0001</v>
       </c>
       <c r="E7" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B7))</f>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D8" s="24" t="str">
         <f>IF(ISNA(B8),NA(),_xll.qlCompositeQuote($E8&amp;"-ResPrem"&amp;QuoteSuffix,E8&amp;QuoteSuffix,C8,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003719918-ResPrem_Quote#0000</v>
+        <v>IT0003719918-ResPrem_Quote#0001</v>
       </c>
       <c r="E8" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B8))</f>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="D9" s="24" t="str">
         <f>IF(ISNA(B9),NA(),_xll.qlCompositeQuote($E9&amp;"-ResPrem"&amp;QuoteSuffix,E9&amp;QuoteSuffix,C9,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003844534-ResPrem_Quote#0000</v>
+        <v>IT0003844534-ResPrem_Quote#0001</v>
       </c>
       <c r="E9" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B9))</f>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="D10" s="24" t="str">
         <f>IF(ISNA(B10),NA(),_xll.qlCompositeQuote($E10&amp;"-ResPrem"&amp;QuoteSuffix,E10&amp;QuoteSuffix,C10,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004019581-ResPrem_Quote#0000</v>
+        <v>IT0004019581-ResPrem_Quote#0001</v>
       </c>
       <c r="E10" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B10))</f>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="D11" s="24" t="str">
         <f>IF(ISNA(B11),NA(),_xll.qlCompositeQuote($E11&amp;"-ResPrem"&amp;QuoteSuffix,E11&amp;QuoteSuffix,C11,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004164775-ResPrem_Quote#0000</v>
+        <v>IT0004164775-ResPrem_Quote#0001</v>
       </c>
       <c r="E11" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B11))</f>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="D12" s="24" t="str">
         <f>IF(ISNA(B12),NA(),_xll.qlCompositeQuote($E12&amp;"-ResPrem"&amp;QuoteSuffix,E12&amp;QuoteSuffix,C12,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003242747-ResPrem_Quote#0000</v>
+        <v>IT0003242747-ResPrem_Quote#0001</v>
       </c>
       <c r="E12" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B12))</f>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="D13" s="24" t="str">
         <f>IF(ISNA(B13),NA(),_xll.qlCompositeQuote($E13&amp;"-ResPrem"&amp;QuoteSuffix,E13&amp;QuoteSuffix,C13,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004273493-ResPrem_Quote#0000</v>
+        <v>IT0004273493-ResPrem_Quote#0001</v>
       </c>
       <c r="E13" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B13))</f>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="D14" s="24" t="str">
         <f>IF(ISNA(B14),NA(),_xll.qlCompositeQuote($E14&amp;"-ResPrem"&amp;QuoteSuffix,E14&amp;QuoteSuffix,C14,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004361041-ResPrem_Quote#0000</v>
+        <v>IT0004361041-ResPrem_Quote#0001</v>
       </c>
       <c r="E14" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B14))</f>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="D15" s="24" t="str">
         <f>IF(ISNA(B15),NA(),_xll.qlCompositeQuote($E15&amp;"-ResPrem"&amp;QuoteSuffix,E15&amp;QuoteSuffix,C15,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003493258-ResPrem_Quote#0000</v>
+        <v>IT0003493258-ResPrem_Quote#0001</v>
       </c>
       <c r="E15" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B15))</f>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D16" s="24" t="str">
         <f>IF(ISNA(B16),NA(),_xll.qlCompositeQuote($E16&amp;"-ResPrem"&amp;QuoteSuffix,E16&amp;QuoteSuffix,C16,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003644769-ResPrem_Quote#0000</v>
+        <v>IT0003644769-ResPrem_Quote#0001</v>
       </c>
       <c r="E16" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B16))</f>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="D17" s="24" t="str">
         <f>IF(ISNA(B17),NA(),_xll.qlCompositeQuote($E17&amp;"-ResPrem"&amp;QuoteSuffix,E17&amp;QuoteSuffix,C17,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004009673-ResPrem_Quote#0000</v>
+        <v>IT0004009673-ResPrem_Quote#0001</v>
       </c>
       <c r="E17" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B17))</f>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="D18" s="24" t="str">
         <f>IF(ISNA(B18),NA(),_xll.qlCompositeQuote($E18&amp;"-ResPrem"&amp;QuoteSuffix,E18&amp;QuoteSuffix,C18,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004356843-ResPrem_Quote#0000</v>
+        <v>IT0004356843-ResPrem_Quote#0001</v>
       </c>
       <c r="E18" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B18))</f>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="D19" s="24" t="str">
         <f>IF(ISNA(B19),NA(),_xll.qlCompositeQuote($E19&amp;"-ResPrem"&amp;QuoteSuffix,E19&amp;QuoteSuffix,C19,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003256820-ResPrem_Quote#0000</v>
+        <v>IT0003256820-ResPrem_Quote#0001</v>
       </c>
       <c r="E19" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B19))</f>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="D20" s="24" t="str">
         <f>IF(ISNA(B20),NA(),_xll.qlCompositeQuote($E20&amp;"-ResPrem"&amp;QuoteSuffix,E20&amp;QuoteSuffix,C20,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003535157-ResPrem_Quote#0000</v>
+        <v>IT0003535157-ResPrem_Quote#0001</v>
       </c>
       <c r="E20" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B20))</f>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D21" s="24" t="str">
         <f>IF(ISNA(B21),NA(),_xll.qlCompositeQuote($E21&amp;"-ResPrem"&amp;QuoteSuffix,E21&amp;QuoteSuffix,C21,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0003934657-ResPrem_Quote#0000</v>
+        <v>IT0003934657-ResPrem_Quote#0001</v>
       </c>
       <c r="E21" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B21))</f>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="D22" s="24" t="str">
         <f>IF(ISNA(B22),NA(),_xll.qlCompositeQuote($E22&amp;"-ResPrem"&amp;QuoteSuffix,E22&amp;QuoteSuffix,C22,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0004286966-ResPrem_Quote#0000</v>
+        <v>IT0004286966-ResPrem_Quote#0001</v>
       </c>
       <c r="E22" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B22))</f>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="F23" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D23)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G23" s="23"/>
     </row>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="F24" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D24)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G24" s="23"/>
     </row>
@@ -1655,6 +1655,12 @@
       <c r="E25" s="36"/>
       <c r="F25" s="35"/>
       <c r="G25" s="25"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="28" t="str">
+        <f>_xll.ohObjectCallerAddress("Residues"&amp;B1)</f>
+        <v>'[EUR_ITALY.xlsx]BTP Strip Feb-Aug'!R28C13</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1716,9 +1722,9 @@
       <c r="E2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="31" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>#NAME?</v>
+      <c r="F2" s="31" t="str">
+        <f>_xll.ohRangeRetrieveError(D2)</f>
+        <v/>
       </c>
       <c r="G2" s="23"/>
     </row>
@@ -1734,7 +1740,7 @@
       </c>
       <c r="D3" s="24" t="str">
         <f>IF(ISNA(B3),NA(),_xll.qlCompositeQuote($E3&amp;"-ResPrem"&amp;QuoteSuffix,E3&amp;QuoteSuffix,C3,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0001448619-ResPrem_Quote#0000</v>
+        <v>IT0001448619-ResPrem_Quote#0001</v>
       </c>
       <c r="E3" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B3))</f>
@@ -1757,7 +1763,7 @@
       </c>
       <c r="D4" s="24" t="str">
         <f>IF(ISNA(B4),NA(),_xll.qlCompositeQuote($E4&amp;"-ResPrem"&amp;QuoteSuffix,E4&amp;QuoteSuffix,C4,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0000366655-ResPrem_Quote#0000</v>
+        <v>IT0000366655-ResPrem_Quote#0001</v>
       </c>
       <c r="E4" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B4))</f>
@@ -1780,7 +1786,7 @@
       </c>
       <c r="D5" s="24" t="str">
         <f>IF(ISNA(B5),NA(),_xll.qlCompositeQuote($E5&amp;"-ResPrem"&amp;QuoteSuffix,E5&amp;QuoteSuffix,C5,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0001086567-ResPrem_Quote#0000</v>
+        <v>IT0001086567-ResPrem_Quote#0001</v>
       </c>
       <c r="E5" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B5))</f>
@@ -1803,7 +1809,7 @@
       </c>
       <c r="D6" s="24" t="str">
         <f>IF(ISNA(B6),NA(),_xll.qlCompositeQuote($E6&amp;"-ResPrem"&amp;QuoteSuffix,E6&amp;QuoteSuffix,C6,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0001174611-ResPrem_Quote#0000</v>
+        <v>IT0001174611-ResPrem_Quote#0001</v>
       </c>
       <c r="E6" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B6))</f>
@@ -1826,7 +1832,7 @@
       </c>
       <c r="D7" s="24" t="str">
         <f>IF(ISNA(B7),NA(),_xll.qlCompositeQuote($E7&amp;"-ResPrem"&amp;QuoteSuffix,E7&amp;QuoteSuffix,C7,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0001278511-ResPrem_Quote#0000</v>
+        <v>IT0001278511-ResPrem_Quote#0001</v>
       </c>
       <c r="E7" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B7))</f>
@@ -1849,7 +1855,7 @@
       </c>
       <c r="D8" s="24" t="str">
         <f>IF(ISNA(B8),NA(),_xll.qlCompositeQuote($E8&amp;"-ResPrem"&amp;QuoteSuffix,E8&amp;QuoteSuffix,C8,"-",Permanent,Trigger,ObjectOverwrite))</f>
-        <v>IT0001444378-ResPrem_Quote#0000</v>
+        <v>IT0001444378-ResPrem_Quote#0001</v>
       </c>
       <c r="E8" s="24" t="str">
         <f>_xll.qlBondMaturityLookup("StrippableBTPs",_xll.qlBondMaturityDate(B8))</f>
@@ -1880,7 +1886,7 @@
       </c>
       <c r="F9" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D9)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G9" s="23"/>
     </row>
@@ -1903,7 +1909,7 @@
       </c>
       <c r="F10" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D10)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G10" s="23"/>
     </row>
@@ -1926,7 +1932,7 @@
       </c>
       <c r="F11" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D11)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G11" s="23"/>
     </row>
@@ -1949,7 +1955,7 @@
       </c>
       <c r="F12" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D12)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G12" s="23"/>
     </row>
@@ -1972,7 +1978,7 @@
       </c>
       <c r="F13" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D13)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G13" s="23"/>
     </row>
@@ -1995,7 +2001,7 @@
       </c>
       <c r="F14" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D14)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G14" s="23"/>
     </row>
@@ -2018,7 +2024,7 @@
       </c>
       <c r="F15" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D15)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G15" s="23"/>
     </row>
@@ -2041,7 +2047,7 @@
       </c>
       <c r="F16" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D16)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G16" s="23"/>
     </row>
@@ -2064,7 +2070,7 @@
       </c>
       <c r="F17" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D17)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G17" s="23"/>
     </row>
@@ -2087,7 +2093,7 @@
       </c>
       <c r="F18" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D18)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G18" s="23"/>
     </row>
@@ -2110,7 +2116,7 @@
       </c>
       <c r="F19" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D19)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G19" s="23"/>
     </row>
@@ -2133,7 +2139,7 @@
       </c>
       <c r="F20" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D20)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G20" s="23"/>
     </row>
@@ -2156,7 +2162,7 @@
       </c>
       <c r="F21" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D21)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G21" s="23"/>
     </row>
@@ -2179,7 +2185,7 @@
       </c>
       <c r="F22" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D22)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G22" s="23"/>
     </row>
@@ -2202,7 +2208,7 @@
       </c>
       <c r="F23" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D23)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G23" s="23"/>
     </row>
@@ -2225,7 +2231,7 @@
       </c>
       <c r="F24" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D24)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G24" s="23"/>
     </row>
@@ -2295,9 +2301,9 @@
       <c r="E2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="31" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>#NAME?</v>
+      <c r="F2" s="31" t="str">
+        <f>_xll.ohRangeRetrieveError(D2)</f>
+        <v/>
       </c>
       <c r="G2" s="23"/>
     </row>
@@ -2320,7 +2326,7 @@
       </c>
       <c r="F3" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D3)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G3" s="23"/>
     </row>
@@ -2342,7 +2348,7 @@
       </c>
       <c r="F4" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D4)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G4" s="23"/>
     </row>
@@ -2364,7 +2370,7 @@
       </c>
       <c r="F5" s="39" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D5)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="G5" s="23"/>
     </row>

</xml_diff>